<commit_message>
基本完成数据收集的预研 Signed-off-by: unknown <wendemo@163.com>
</commit_message>
<xml_diff>
--- a/doc/定量仪软件功能梳理V1.0.xlsx
+++ b/doc/定量仪软件功能梳理V1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="功能梳理" sheetId="1" r:id="rId1"/>
@@ -311,24 +311,30 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,7 +886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -906,7 +912,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -916,7 +922,7 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -924,7 +930,7 @@
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -934,7 +940,7 @@
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -942,7 +948,7 @@
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -950,7 +956,7 @@
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -958,7 +964,7 @@
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
@@ -966,76 +972,76 @@
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="5"/>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="4" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1089,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1101,68 +1107,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="B3" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="162">
-      <c r="A8" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" ht="148.5">
+      <c r="A8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="C9" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>